<commit_message>
change code for 12/13 presentation
</commit_message>
<xml_diff>
--- a/PSG_sleep_index_20220928.xlsx
+++ b/PSG_sleep_index_20220928.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luhaoyu/Documents/research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A86DF7C-0217-3B4E-8BC0-17A7E14364E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B3F2A8-29AE-5746-8D85-509690A4F1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{435C2B69-2017-4921-9724-291180F2038E}"/>
   </bookViews>
@@ -2969,8 +2969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF4102E9-7D08-485C-9109-3AFE3B69255E}">
   <dimension ref="A1:AD310"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A272" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AD1" sqref="AD1"/>
     </sheetView>
   </sheetViews>

</xml_diff>